<commit_message>
modify raw data file to correct data entry error at line 120
</commit_message>
<xml_diff>
--- a/nectar analysis/raw data/2015 Balsamroot Nectar Data raw.xlsx
+++ b/nectar analysis/raw data/2015 Balsamroot Nectar Data raw.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Audrey McCombs\Desktop\EEB 590\MAL\nectar analysis\raw data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="132" windowWidth="20112" windowHeight="7932"/>
   </bookViews>
@@ -278,6 +283,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -325,7 +333,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -360,7 +368,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -571,9 +579,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S142" sqref="S142"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5362,8 +5370,20 @@
       <c r="H121" t="s">
         <v>20</v>
       </c>
+      <c r="I121">
+        <v>2</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+      <c r="N121">
+        <v>1</v>
+      </c>
       <c r="O121">
         <v>55</v>
+      </c>
+      <c r="P121">
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>